<commit_message>
Directory changes : new configuration to accomodate C-Programming DSA
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimal\eclipse-workspace\anujSirDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE554023-F630-4353-843B-24C209F42109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A622431-2D44-4B92-B27F-99273D78B77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>